<commit_message>
Further tweaks and start building spreadsheet read me
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B9EF7-62CC-5044-AEAD-1318C891A583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4190B80-0537-5F47-A144-138AC6BA718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33660" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
     <sheet name="soa" sheetId="1" r:id="rId4"/>
+    <sheet name="ReadMe" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="153">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -464,14 +465,50 @@
     <t>organisationAddress</t>
   </si>
   <si>
-    <t>Gartenstrasse 9| Basel||| 4052|CHE</t>
+    <t>Gartenstrasse 9| Basel||| 4052|CH</t>
+  </si>
+  <si>
+    <t>studyIdentifiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The orgnaisation address formated using a pipe delimited form:
+line|city|district|state|postal_code|&lt;country code&gt;
+All fields are free text except for &lt;country code&gt;. &lt;country code&gt; is either a two caracter or three character ISO-3166 country code.
+</t>
+  </si>
+  <si>
+    <t>Set to either 'registry', 'sponsor' or 'regulatory'</t>
+  </si>
+  <si>
+    <t>String identifier</t>
+  </si>
+  <si>
+    <t>String name</t>
+  </si>
+  <si>
+    <t>Organisation identifier, a string</t>
+  </si>
+  <si>
+    <t>The scheme for the organisation identifier. Example would be 'DUNS'</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>String title</t>
+  </si>
+  <si>
+    <t>String version</t>
+  </si>
+  <si>
+    <t>CDISC code in the form &lt;C code&gt;=&lt;decode (preferred term)&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -516,8 +553,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -527,6 +572,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -598,6 +649,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5395,4 +5456,163 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814FDBDD-6B5B-594E-9925-640D6E03C7E7}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="127.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="24"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add in better CDISC CT handling for specific fields
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4190B80-0537-5F47-A144-138AC6BA718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4DD04B-EDA0-844B-8014-B5734BAEC2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -345,12 +345,6 @@
     <t>studyPhase</t>
   </si>
   <si>
-    <t>C98388=Interventional Study</t>
-  </si>
-  <si>
-    <t>C15602=Phase III Trial</t>
-  </si>
-  <si>
     <t>Tocilizumab in Patients With Severe COVID-19 Pneumonia</t>
   </si>
   <si>
@@ -502,6 +496,12 @@
   </si>
   <si>
     <t>CDISC code in the form &lt;C code&gt;=&lt;decode (preferred term)&gt;</t>
+  </si>
+  <si>
+    <t>Interventional</t>
+  </si>
+  <si>
+    <t>Phase III Trial</t>
   </si>
 </sst>
 </file>
@@ -635,21 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -659,6 +644,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="10">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1037,76 +1037,76 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1133,69 +1133,69 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+        <v>121</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+        <v>123</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+        <v>125</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+        <v>127</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+        <v>129</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+        <v>131</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1207,7 +1207,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>42</v>
@@ -1224,42 +1224,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1298,10 +1298,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1311,49 +1311,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20" t="s">
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="20"/>
+      <c r="AL1" s="24"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1464,8 +1464,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1576,8 +1576,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -1688,8 +1688,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1800,8 +1800,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -1908,12 +1908,12 @@
         <v>83</v>
       </c>
       <c r="AL6" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2024,8 +2024,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -5462,7 +5462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814FDBDD-6B5B-594E-9925-640D6E03C7E7}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -5473,45 +5473,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="16" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -5519,61 +5519,61 @@
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="24"/>
+      <c r="A8" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="B12" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="B13" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>108</v>
-      </c>
       <c r="B14" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="89" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>140</v>
+      <c r="A15" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
First cut for endpoint and objectives
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A28AB6A-9B9C-6E4F-A0D6-B400F6D713C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB65767-C227-0C49-93F0-EC063FDAA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="studyDesignII" sheetId="6" r:id="rId5"/>
     <sheet name="ReadMe" sheetId="5" r:id="rId6"/>
     <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="199">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -574,6 +575,75 @@
   </si>
   <si>
     <t>80 years</t>
+  </si>
+  <si>
+    <t>The primary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia</t>
+  </si>
+  <si>
+    <t>Clinical status assessed using a 7-category ordinal scale at Day 28</t>
+  </si>
+  <si>
+    <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia</t>
+  </si>
+  <si>
+    <t>Time to improvement of at least 2 categories relative to baseline on a 7-category ordinal scale of clinical status</t>
+  </si>
+  <si>
+    <t>Incidence of mechanical ventilation</t>
+  </si>
+  <si>
+    <t>Ventilator-free days to Day 28</t>
+  </si>
+  <si>
+    <t>Incidence of intensive care unit (ICU) stay</t>
+  </si>
+  <si>
+    <t>Duration of ICU stay</t>
+  </si>
+  <si>
+    <t>Time to clinical failure, defined as the time to death, mechanical ventilation, ICU admission, or withdrawal (whichever occurs first). For patients entering the study already in ICU or on mechanical ventilation, clinical failure is defined as a one-category worsening on the ordinal scale, withdrawal or death.</t>
+  </si>
+  <si>
+    <t>Mortality rate at Days 7, 14, 21, 28, and 60</t>
+  </si>
+  <si>
+    <t>Duration of supplemental oxygen</t>
+  </si>
+  <si>
+    <t>objectiveDescription</t>
+  </si>
+  <si>
+    <t>objectiveLevel</t>
+  </si>
+  <si>
+    <t>endpointDescription</t>
+  </si>
+  <si>
+    <t>endpointPurposeDescription</t>
+  </si>
+  <si>
+    <t>endpointLevel</t>
+  </si>
+  <si>
+    <t>Time to hospital discharge or “ready for discharge” (as evidenced by normal body temperature and respiratory rate, and stable oxygen saturation on ambient air or &lt;= 2L supplemental oxygen)</t>
+  </si>
+  <si>
+    <t>Time to clinical improvement (TTCI) defined as a National Early Warning Score 2 (NEWS2) of &lt;=2 maintained for 24 hours</t>
+  </si>
+  <si>
+    <t>Time to recovery, defined as discharged or “ready for discharge” (as evidenced by normal body temperature and respiratory rate, and stable oxygen saturation on ambient air or &lt;= 2L supplemental oxygen); OR, in a non-ICU hospital ward (or “ready for hospital ward”) not requiring supplemental oxygen</t>
+  </si>
+  <si>
+    <t>Primary Endpoint</t>
+  </si>
+  <si>
+    <t>Study Primary Objective</t>
+  </si>
+  <si>
+    <t>Study Secondary Objective</t>
+  </si>
+  <si>
+    <t>Secondary Enpoint</t>
   </si>
 </sst>
 </file>
@@ -666,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -731,6 +801,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5782,7 +5855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -5832,4 +5905,737 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
+  <dimension ref="A1:P36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="59.5" customWidth="1"/>
+    <col min="4" max="5" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix error in Roche study
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8F86A-70A7-7E45-B11F-81450924A44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D33E2A-7C6E-A149-B386-0BA1C3204148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="500" windowWidth="32140" windowHeight="23720" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4940" yWindow="500" windowWidth="53040" windowHeight="25840" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="214">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -321,15 +321,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>BC:Age</t>
-  </si>
-  <si>
-    <t>BC:Sex</t>
-  </si>
-  <si>
-    <t>BC:Race</t>
-  </si>
-  <si>
     <t>BC:Respiratory rate, BC:Pulse rate, BC:Systolic blood pressure, BC:Diastolic blood pressure, BC:Body temperature, BC:Oxygen saturation, BC:NEWS2</t>
   </si>
   <si>
@@ -691,6 +682,9 @@
   </si>
   <si>
     <t>END12</t>
+  </si>
+  <si>
+    <t>BC:Age, BC:Sex, BC:Race</t>
   </si>
 </sst>
 </file>
@@ -1174,30 +1168,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" s="10">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1221,76 +1215,76 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
         <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1317,10 +1311,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1328,10 +1322,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1339,10 +1333,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1350,10 +1344,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -1361,10 +1355,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -1372,10 +1366,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -1391,7 +1385,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>42</v>
@@ -1408,42 +1402,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1461,13 +1455,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
-  <dimension ref="A1:AO38"/>
+  <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="AG10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AL6" sqref="AL6"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2092,7 +2086,7 @@
         <v>83</v>
       </c>
       <c r="AL6" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
@@ -2512,7 +2506,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>213</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -2624,14 +2618,17 @@
       <c r="A13" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>93</v>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>91</v>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>91</v>
@@ -2737,14 +2734,17 @@
       <c r="A14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>94</v>
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>91</v>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>91</v>
@@ -2851,16 +2851,16 @@
         <v>91</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>91</v>
@@ -2967,7 +2967,7 @@
         <v>91</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>91</v>
@@ -3083,7 +3083,7 @@
         <v>91</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>91</v>
@@ -3199,16 +3199,16 @@
         <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>91</v>
@@ -3219,8 +3219,8 @@
       <c r="H18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>91</v>
+      <c r="I18" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>91</v>
@@ -3297,17 +3297,17 @@
       <c r="AH18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AI18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL18" s="2" t="s">
-        <v>91</v>
+      <c r="AI18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.2">
@@ -3315,7 +3315,7 @@
         <v>91</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>91</v>
@@ -3431,7 +3431,7 @@
         <v>91</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>91</v>
@@ -3451,8 +3451,8 @@
       <c r="H20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>12</v>
+      <c r="I20" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>91</v>
@@ -3529,17 +3529,17 @@
       <c r="AH20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AI20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL20" s="1" t="s">
-        <v>12</v>
+      <c r="AI20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.2">
@@ -3547,7 +3547,7 @@
         <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>91</v>
@@ -3567,83 +3567,83 @@
       <c r="H21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH21" s="2" t="s">
-        <v>91</v>
+      <c r="I21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="AI21" s="2" t="s">
         <v>91</v>
@@ -3654,8 +3654,8 @@
       <c r="AK21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AL21" s="2" t="s">
-        <v>91</v>
+      <c r="AL21" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
@@ -3663,7 +3663,7 @@
         <v>91</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>91</v>
@@ -3671,223 +3671,223 @@
       <c r="D22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AI22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK22" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>91</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK23" s="2" t="s">
-        <v>91</v>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
@@ -3895,25 +3895,25 @@
         <v>91</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>12</v>
+      <c r="D24" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
+      <c r="F24" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>12</v>
+      <c r="H24" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>12</v>
@@ -4006,108 +4006,108 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>12</v>
+      <c r="F25" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH25" s="2" t="s">
-        <v>91</v>
+      <c r="H25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="AI25" s="1" t="s">
         <v>12</v>
@@ -4127,7 +4127,7 @@
         <v>91</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>91</v>
@@ -4243,13 +4243,13 @@
         <v>91</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>91</v>
+      <c r="D27" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -4266,77 +4266,77 @@
       <c r="I27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>12</v>
+      <c r="J27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>12</v>
+      <c r="N27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>12</v>
+      <c r="Q27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="T27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z27" s="1" t="s">
-        <v>12</v>
+      <c r="U27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AA27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG27" s="1" t="s">
-        <v>12</v>
+      <c r="AB27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG27" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AH27" s="1" t="s">
         <v>12</v>
@@ -4351,7 +4351,7 @@
         <v>12</v>
       </c>
       <c r="AL27" s="1" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.2">
@@ -4359,13 +4359,13 @@
         <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>91</v>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
@@ -4382,77 +4382,77 @@
       <c r="I28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>12</v>
+      <c r="J28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>12</v>
+      <c r="N28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>12</v>
+      <c r="Q28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z28" s="1" t="s">
-        <v>12</v>
+      <c r="U28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AA28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG28" s="1" t="s">
-        <v>12</v>
+      <c r="AB28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG28" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AH28" s="1" t="s">
         <v>12</v>
@@ -4475,13 +4475,13 @@
         <v>91</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>12</v>
+      <c r="D29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -4489,14 +4489,14 @@
       <c r="F29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>12</v>
+      <c r="G29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>12</v>
+      <c r="I29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>91</v>
@@ -4507,8 +4507,8 @@
       <c r="L29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>12</v>
+      <c r="M29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>91</v>
@@ -4516,8 +4516,8 @@
       <c r="O29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>12</v>
+      <c r="P29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>91</v>
@@ -4528,8 +4528,8 @@
       <c r="S29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="T29" s="1" t="s">
-        <v>12</v>
+      <c r="T29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>91</v>
@@ -4549,8 +4549,8 @@
       <c r="Z29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AA29" s="1" t="s">
-        <v>12</v>
+      <c r="AA29" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AB29" s="2" t="s">
         <v>91</v>
@@ -4570,46 +4570,46 @@
       <c r="AG29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AH29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL29" s="1" t="s">
-        <v>76</v>
+      <c r="AH29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL29" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>91</v>
+      <c r="A30" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
+      <c r="D30" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>91</v>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>91</v>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>12</v>
@@ -4632,8 +4632,8 @@
       <c r="O30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>12</v>
+      <c r="P30" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>91</v>
@@ -4692,8 +4692,8 @@
       <c r="AI30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AJ30" s="1" t="s">
-        <v>12</v>
+      <c r="AJ30" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AK30" s="1" t="s">
         <v>12</v>
@@ -4707,7 +4707,7 @@
         <v>91</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>91</v>
@@ -4718,14 +4718,14 @@
       <c r="E31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>91</v>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>91</v>
@@ -4739,8 +4739,8 @@
       <c r="L31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M31" s="2" t="s">
-        <v>91</v>
+      <c r="M31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>91</v>
@@ -4760,8 +4760,8 @@
       <c r="S31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="T31" s="2" t="s">
-        <v>91</v>
+      <c r="T31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>91</v>
@@ -4781,8 +4781,8 @@
       <c r="Z31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AA31" s="2" t="s">
-        <v>91</v>
+      <c r="AA31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="AB31" s="2" t="s">
         <v>91</v>
@@ -4802,28 +4802,28 @@
       <c r="AG31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AH31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AI31" s="2" t="s">
-        <v>91</v>
+      <c r="AH31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="AJ31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AK31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL31" s="2" t="s">
-        <v>91</v>
+      <c r="AK31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL31" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>34</v>
+      <c r="A32" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>91</v>
@@ -4834,14 +4834,14 @@
       <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
+      <c r="F32" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>12</v>
+      <c r="H32" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>12</v>
@@ -4939,7 +4939,7 @@
         <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>91</v>
@@ -4950,26 +4950,26 @@
       <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
+      <c r="F33" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>91</v>
+      <c r="H33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>12</v>
@@ -4980,8 +4980,8 @@
       <c r="O33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>91</v>
+      <c r="P33" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>91</v>
@@ -5037,8 +5037,8 @@
       <c r="AH33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AI33" s="1" t="s">
-        <v>12</v>
+      <c r="AI33" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AJ33" s="2" t="s">
         <v>91</v>
@@ -5055,7 +5055,7 @@
         <v>91</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>91</v>
@@ -5069,14 +5069,14 @@
       <c r="F34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>12</v>
+      <c r="G34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>12</v>
+      <c r="I34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>91</v>
@@ -5087,8 +5087,8 @@
       <c r="L34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>12</v>
+      <c r="M34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>91</v>
@@ -5108,8 +5108,8 @@
       <c r="S34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="T34" s="1" t="s">
-        <v>12</v>
+      <c r="T34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="U34" s="2" t="s">
         <v>91</v>
@@ -5129,8 +5129,8 @@
       <c r="Z34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AA34" s="1" t="s">
-        <v>12</v>
+      <c r="AA34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AB34" s="2" t="s">
         <v>91</v>
@@ -5153,14 +5153,14 @@
       <c r="AH34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AI34" s="1" t="s">
-        <v>12</v>
+      <c r="AI34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AJ34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AK34" s="1" t="s">
-        <v>12</v>
+      <c r="AK34" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AL34" s="1" t="s">
         <v>12</v>
@@ -5171,7 +5171,7 @@
         <v>91</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>91</v>
@@ -5194,17 +5194,17 @@
       <c r="I35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>12</v>
+      <c r="J35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>91</v>
@@ -5212,8 +5212,8 @@
       <c r="O35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P35" s="1" t="s">
-        <v>12</v>
+      <c r="P35" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>91</v>
@@ -5275,8 +5275,8 @@
       <c r="AJ35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AK35" s="1" t="s">
-        <v>12</v>
+      <c r="AK35" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="AL35" s="1" t="s">
         <v>12</v>
@@ -5287,7 +5287,7 @@
         <v>91</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>91</v>
@@ -5307,8 +5307,8 @@
       <c r="H36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>91</v>
+      <c r="I36" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>91</v>
@@ -5319,8 +5319,8 @@
       <c r="L36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M36" s="2" t="s">
-        <v>91</v>
+      <c r="M36" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>91</v>
@@ -5395,238 +5395,6 @@
         <v>91</v>
       </c>
       <c r="AL36" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="U38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL38" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5659,72 +5427,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -5751,36 +5519,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>160</v>
-      </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -5807,25 +5575,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>173</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -5833,22 +5601,22 @@
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>184</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5856,22 +5624,22 @@
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5881,14 +5649,14 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -5898,14 +5666,14 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -5915,14 +5683,14 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -5932,14 +5700,14 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -5949,14 +5717,14 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -5966,14 +5734,14 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5983,14 +5751,14 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -6000,14 +5768,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -6017,14 +5785,14 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -6034,14 +5802,14 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6309,7 +6077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -6325,54 +6093,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak titles in Roche study setup
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7383AF8-71A0-4744-BA40-7626F51AF734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0591F80-10E7-A842-80C8-86D39879184A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="230">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -723,10 +723,16 @@
     <t>final</t>
   </si>
   <si>
-    <t>A RANDOMIZED, DOUBLE-BLIND, PLACEBOCONTROLLED, MULTICENTER STUDY TO EVALUATE THE SAFETY AND EFFICACY OF TOCILIZUMAB IN PATIENTS WITH SEVERE COVID-19 PNEUMONIA</t>
-  </si>
-  <si>
     <t>Tocilizumab</t>
+  </si>
+  <si>
+    <t>COVACTA</t>
+  </si>
+  <si>
+    <t>A Randomized, Double-Blind, Placebo-Controlled, Multicenter Study to Evaluate the Safety and Efficacy of Tocilizumab in Patients With Severe COVID-19 Pneumonia</t>
+  </si>
+  <si>
+    <t>A Study to Evaluate the Safety and Efficacy of Tocilizumab in Patients With Severe COVID-19 Pneumonia (COVACTA)</t>
   </si>
 </sst>
 </file>
@@ -819,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -883,6 +889,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -898,14 +913,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,14 +1233,14 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="98.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="7" width="21.1640625" customWidth="1"/>
@@ -1274,7 +1283,9 @@
       <c r="A5" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
@@ -1297,73 +1308,79 @@
       <c r="D8" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="24" t="s">
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="B9" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>229</v>
+      </c>
       <c r="D9" s="20"/>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="31">
+      <c r="G9" s="26">
         <v>43908</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B10" s="24" t="s">
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="B10" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>229</v>
+      </c>
       <c r="D10" s="20"/>
       <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="31">
+      <c r="G10" s="26">
         <v>43935</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="B11" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>229</v>
+      </c>
       <c r="D11" s="20"/>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="31">
+      <c r="G11" s="26">
         <v>43993</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1489,67 +1506,67 @@
       <c r="A1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1652,10 +1669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1665,49 +1682,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29" t="s">
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="29"/>
+      <c r="AL1" s="32"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1818,8 +1835,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1930,8 +1947,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2042,8 +2059,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2154,8 +2171,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2266,8 +2283,8 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2378,8 +2395,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Add in support for business therapeutic areas
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0591F80-10E7-A842-80C8-86D39879184A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034204C-CBFB-D94F-8F5E-61B920117AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="232">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>A Study to Evaluate the Safety and Efficacy of Tocilizumab in Patients With Severe COVID-19 Pneumonia (COVACTA)</t>
+  </si>
+  <si>
+    <t>businessTherapeuticAreas</t>
+  </si>
+  <si>
+    <t>SPONSOR: PHARMA=Pharma Division</t>
   </si>
 </sst>
 </file>
@@ -898,6 +904,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -912,9 +921,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1295,71 +1301,57 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B9" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C9" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D9" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F9" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G9" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="26">
-        <v>43908</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="28" t="s">
         <v>229</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="26">
-        <v>43935</v>
+        <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>225</v>
@@ -1369,21 +1361,43 @@
       <c r="A11" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="28" t="s">
         <v>229</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="26">
+        <v>43935</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="26">
         <v>43993</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1506,67 +1520,67 @@
       <c r="A1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1669,10 +1683,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1682,49 +1696,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32" t="s">
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="32"/>
+      <c r="AL1" s="33"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1835,8 +1849,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1947,8 +1961,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2059,8 +2073,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2171,8 +2185,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2283,8 +2297,8 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2395,8 +2409,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Improve CT in Study Design sheet
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034204C-CBFB-D94F-8F5E-61B920117AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820EC1D9-B2BC-244F-A2A4-02EEDAFFBC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -414,27 +414,15 @@
     <t>studyDesignBlindingScheme</t>
   </si>
   <si>
-    <t>C49659=OPEN LABEL</t>
-  </si>
-  <si>
     <t>trialIntentTypes</t>
   </si>
   <si>
-    <t>C15714=BASIC SCIENCE, C139174=DEVICE FEASIBILITY</t>
-  </si>
-  <si>
     <t>trialTypes</t>
   </si>
   <si>
-    <t>C12345=Observational</t>
-  </si>
-  <si>
     <t>interventionModel</t>
   </si>
   <si>
-    <t>C12346=None</t>
-  </si>
-  <si>
     <t xml:space="preserve">Screening </t>
   </si>
   <si>
@@ -739,6 +727,18 @@
   </si>
   <si>
     <t>SPONSOR: PHARMA=Pharma Division</t>
+  </si>
+  <si>
+    <t>OPEN LABEL</t>
+  </si>
+  <si>
+    <t>BASIC SCIENCE,    DEVICE FEASIBILITY</t>
+  </si>
+  <si>
+    <t>Efficacy Study</t>
+  </si>
+  <si>
+    <t>C82639</t>
   </si>
 </sst>
 </file>
@@ -783,14 +783,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,6 +795,14 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -831,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -860,9 +860,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -876,10 +873,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -901,26 +898,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1254,151 +1251,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>137</v>
+      <c r="B3" s="21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>138</v>
+      <c r="B4" s="21" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="E9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="F9" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="G9" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="H9" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="25" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="G9" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="H9" s="25" t="s">
+      <c r="B10" s="27" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D10" s="20"/>
+      <c r="C10" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="20"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>43935</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <v>43993</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1437,7 +1434,7 @@
         <v>103</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,7 +1488,7 @@
         <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1506,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1514,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="30" t="s">
@@ -1528,7 +1525,7 @@
       <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B2" s="31" t="s">
@@ -1539,48 +1536,48 @@
       <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="6" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
       <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B5" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="B6" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1591,60 +1588,60 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>131</v>
+      <c r="A9" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>131</v>
+      <c r="A10" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1683,10 +1680,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1696,49 +1693,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33" t="s">
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="33"/>
+      <c r="AL1" s="29"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1849,8 +1846,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1961,8 +1958,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2073,8 +2070,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2185,8 +2182,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2292,13 +2289,13 @@
       <c r="AK6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AL6" s="15" t="s">
-        <v>134</v>
+      <c r="AL6" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2409,8 +2406,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2713,7 +2710,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -5633,73 +5630,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>141</v>
+      <c r="A1" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
         <v>142</v>
       </c>
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
         <v>142</v>
       </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
       <c r="D5" s="11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -5725,37 +5722,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -5781,72 +5778,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>173</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>200</v>
+      <c r="A2" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>201</v>
+      <c r="A3" s="19" t="s">
+        <v>197</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5856,14 +5853,14 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -5873,14 +5870,14 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -5890,14 +5887,14 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -5907,14 +5904,14 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -5924,14 +5921,14 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -5941,14 +5938,14 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5958,14 +5955,14 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -5975,14 +5972,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -5992,14 +5989,14 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -6009,14 +6006,14 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6299,55 +6296,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="A1" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="C1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>189</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all examples for configuration update
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820EC1D9-B2BC-244F-A2A4-02EEDAFFBC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9428CD07-4D7E-5E40-9CB6-BD084578ABA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="study" sheetId="2" r:id="rId1"/>
-    <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
-    <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
-    <sheet name="soa" sheetId="1" r:id="rId4"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId5"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId6"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId7"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId8"/>
+    <sheet name="configuration" sheetId="10" r:id="rId1"/>
+    <sheet name="study" sheetId="2" r:id="rId2"/>
+    <sheet name="studyIdentifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="studyDesign" sheetId="4" r:id="rId4"/>
+    <sheet name="soa" sheetId="1" r:id="rId5"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId6"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="235">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -739,6 +740,15 @@
   </si>
   <si>
     <t>C82639</t>
+  </si>
+  <si>
+    <t>CT Version</t>
+  </si>
+  <si>
+    <t>SNOMED=January 31, 2018</t>
+  </si>
+  <si>
+    <t>SPONSOR =   12</t>
   </si>
 </sst>
 </file>
@@ -904,11 +914,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -916,8 +923,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1232,6 +1242,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -1403,7 +1447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1499,11 +1543,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
@@ -1517,67 +1561,67 @@
       <c r="A1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1657,7 +1701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
@@ -1680,10 +1724,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1693,49 +1737,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29" t="s">
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="29"/>
+      <c r="AL1" s="32"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1846,8 +1890,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1958,8 +2002,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2070,8 +2114,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2182,8 +2226,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2294,8 +2338,8 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2406,8 +2450,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -5614,7 +5658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -5704,7 +5748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5760,7 +5804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -6277,7 +6321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Remove use of CDISCCT from study identifiers
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9428CD07-4D7E-5E40-9CB6-BD084578ABA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED9A1D7-6E8C-E843-B555-72F67E3D18CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="10" r:id="rId1"/>
@@ -367,9 +367,6 @@
     <t>ClinicalTrials.gov</t>
   </si>
   <si>
-    <t>Registry</t>
-  </si>
-  <si>
     <t>WA42380</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
     <t>2020-001154-22</t>
   </si>
   <si>
-    <t>Sponsor</t>
-  </si>
-  <si>
     <t>EudraCT</t>
   </si>
   <si>
@@ -749,6 +743,12 @@
   </si>
   <si>
     <t>SPONSOR =   12</t>
+  </si>
+  <si>
+    <t>Study Registry</t>
+  </si>
+  <si>
+    <t>Clinical Study Sponsor</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1256,18 +1256,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" t="s">
         <v>232</v>
-      </c>
-      <c r="B2" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1315,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1323,68 +1323,68 @@
         <v>97</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="E9" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="F9" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="G9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>218</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>224</v>
-      </c>
       <c r="C10" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="1">
@@ -1395,18 +1395,18 @@
         <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>224</v>
-      </c>
       <c r="C11" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="1">
@@ -1417,18 +1417,18 @@
         <v>43935</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>224</v>
-      </c>
       <c r="C12" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="1">
@@ -1439,7 +1439,7 @@
         <v>43993</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1451,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1478,7 +1478,7 @@
         <v>103</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1491,48 +1491,48 @@
       <c r="C2" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>107</v>
+      <c r="D2" t="s">
+        <v>233</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>233</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1559,10 +1559,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -1570,10 +1570,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1603,10 +1603,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -1633,7 +1633,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>42</v>
@@ -1650,42 +1650,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2334,7 +2334,7 @@
         <v>83</v>
       </c>
       <c r="AL6" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
@@ -2754,7 +2754,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -5675,72 +5675,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -5767,36 +5767,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -5823,25 +5823,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>167</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>169</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -5849,22 +5849,22 @@
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5872,22 +5872,22 @@
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5897,14 +5897,14 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -5914,14 +5914,14 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -5931,14 +5931,14 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -5948,14 +5948,14 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -5965,14 +5965,14 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -5982,14 +5982,14 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5999,14 +5999,14 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -6016,14 +6016,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -6033,14 +6033,14 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -6050,14 +6050,14 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6341,54 +6341,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in TA handling
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED9A1D7-6E8C-E843-B555-72F67E3D18CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B97C2-5F7A-9F42-BC33-7B497B759BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="500" windowWidth="47260" windowHeight="25840" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="62640" yWindow="500" windowWidth="38340" windowHeight="25840" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="10" r:id="rId1"/>
@@ -397,9 +397,6 @@
     <t>therapeuticAreas</t>
   </si>
   <si>
-    <t>Not supported yet</t>
-  </si>
-  <si>
     <t>studyDesignRationale</t>
   </si>
   <si>
@@ -749,13 +746,16 @@
   </si>
   <si>
     <t>Clinical Study Sponsor</t>
+  </si>
+  <si>
+    <t>SNOMED: 840539006=Disease caused by Severe acute respiratory syndrome coronavirus 2 (disorder), ICD-10:U07.1 = COVID-19, virus identified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -805,14 +805,6 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -917,9 +909,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -928,6 +917,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,18 +1248,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" t="s">
         <v>230</v>
-      </c>
-      <c r="B1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1307,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1323,68 +1315,68 @@
         <v>97</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>209</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>224</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="G9" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="1">
@@ -1395,18 +1387,18 @@
         <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="1">
@@ -1417,18 +1409,18 @@
         <v>43935</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="1">
@@ -1439,7 +1431,7 @@
         <v>43993</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1478,7 +1470,7 @@
         <v>103</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1492,7 +1484,7 @@
         <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>108</v>
@@ -1509,7 +1501,7 @@
         <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" t="s">
         <v>109</v>
@@ -1526,13 +1518,13 @@
         <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
         <v>107</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1547,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1557,45 +1549,45 @@
     <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+        <v>119</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1603,10 +1595,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -1614,10 +1606,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -1633,7 +1625,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>42</v>
@@ -1650,42 +1642,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1724,10 +1716,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1737,49 +1729,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32" t="s">
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="32"/>
+      <c r="AL1" s="31"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1890,8 +1882,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -2002,8 +1994,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2114,8 +2106,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2226,8 +2218,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2334,12 +2326,12 @@
         <v>83</v>
       </c>
       <c r="AL6" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2450,8 +2442,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2754,7 +2746,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -5662,8 +5654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5675,72 +5667,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
         <v>136</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>136</v>
       </c>
-      <c r="C3" t="s">
-        <v>137</v>
-      </c>
       <c r="D3" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5752,7 +5744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -5767,36 +5759,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
         <v>148</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -5808,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5823,25 +5815,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>166</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>167</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -5849,22 +5841,22 @@
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5872,22 +5864,22 @@
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5897,14 +5889,14 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -5914,14 +5906,14 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -5931,14 +5923,14 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -5948,14 +5940,14 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -5965,14 +5957,14 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -5982,14 +5974,14 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5999,14 +5991,14 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -6016,14 +6008,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -6033,14 +6025,14 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -6050,14 +6042,14 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6325,7 +6317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -6341,54 +6333,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new sheet, upgrade old ones and check
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B97C2-5F7A-9F42-BC33-7B497B759BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947E78F0-BD23-EC41-AB0C-1358D4C92D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62640" yWindow="500" windowWidth="38340" windowHeight="25840" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="62640" yWindow="500" windowWidth="38340" windowHeight="25840" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="10" r:id="rId1"/>
     <sheet name="study" sheetId="2" r:id="rId2"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId3"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId4"/>
-    <sheet name="soa" sheetId="1" r:id="rId5"/>
+    <sheet name="mainTimeline" sheetId="1" r:id="rId5"/>
     <sheet name="studyDesignII" sheetId="6" r:id="rId6"/>
     <sheet name="studyDesignPopulations" sheetId="7" r:id="rId7"/>
     <sheet name="studyDesignOE" sheetId="8" r:id="rId8"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="237">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>SNOMED: 840539006=Disease caused by Severe acute respiratory syndrome coronavirus 2 (disorder), ICD-10:U07.1 = COVID-19, virus identified</t>
+  </si>
+  <si>
+    <t>mainTimeline</t>
+  </si>
+  <si>
+    <t>otherTimelines</t>
   </si>
 </sst>
 </file>
@@ -910,6 +916,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -917,9 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1537,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,34 +1559,34 @@
       <c r="A1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
@@ -1616,72 +1622,94 @@
       <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B11" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D11" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B12" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D12" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -1697,11 +1725,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,10 +1744,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1729,49 +1757,49 @@
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31" t="s">
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="31"/>
+      <c r="AL1" s="32"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1882,8 +1910,8 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="6" t="s">
         <v>87</v>
       </c>
@@ -1994,8 +2022,8 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
@@ -2106,8 +2134,8 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2218,8 +2246,8 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="6" t="s">
         <v>89</v>
       </c>
@@ -2330,8 +2358,8 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2442,8 +2470,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Amend study rationale fields to something meaningful
</commit_message>
<xml_diff>
--- a/source_data/Roche Phase 3 NCT04320615.xlsx
+++ b/source_data/Roche Phase 3 NCT04320615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1304D57-C2C3-E042-AB9D-A8BFFA75E4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA199DC-D980-0546-9095-ADD5F4D817F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="43660" yWindow="3660" windowWidth="33600" windowHeight="19480" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="254">
   <si>
     <t>Epoch</t>
   </si>
@@ -398,9 +398,6 @@
     <t>studyDesignRationale</t>
   </si>
   <si>
-    <t>"Study design rationale put here"</t>
-  </si>
-  <si>
     <t>studyDesignBlindingScheme</t>
   </si>
   <si>
@@ -804,6 +801,12 @@
   </si>
   <si>
     <t>Only do it they have man flu</t>
+  </si>
+  <si>
+    <t>There are currently no drugs licensed for the treatment of patients with COVID-19. Given the results of studies outlined above, TCZ, along with standard of care (SOC) treatment, could provide efficacy, offering the potential to treat COVID-19 in hospitalized populations more effectively than current SOC alone. Extensive safety data have previously been generated on the use of TCZ in other indications. Therefore, placebocontrolled study in combination with SOC to assess safety and efficacy of TCZ in hospitalized patients with severe COVID-19 neumonia is justified to address the high unmet need and burden of disease in this severely ill population.</t>
+  </si>
+  <si>
+    <t>Arms/Epochs</t>
   </si>
 </sst>
 </file>
@@ -973,6 +976,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -984,15 +996,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1321,18 +1324,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" t="s">
         <v>228</v>
-      </c>
-      <c r="B1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1353,54 +1356,54 @@
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24" style="38" customWidth="1"/>
+    <col min="4" max="4" width="24" style="34" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="32" t="s">
         <v>244</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
         <v>246</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>247</v>
-      </c>
-      <c r="C2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" t="s">
         <v>249</v>
       </c>
-      <c r="B3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" t="s">
         <v>251</v>
-      </c>
-      <c r="E3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1451,7 +1454,7 @@
         <v>95</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1459,68 +1462,68 @@
         <v>96</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>207</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>222</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="E9" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="F9" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="G9" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" s="24" t="s">
         <v>215</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>220</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>221</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="1">
@@ -1531,18 +1534,18 @@
         <v>43908</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>220</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>221</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="1">
@@ -1553,18 +1556,18 @@
         <v>43935</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>220</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>221</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="1">
@@ -1575,7 +1578,7 @@
         <v>43993</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1588,7 +1591,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1614,7 +1617,7 @@
         <v>102</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1628,7 +1631,7 @@
         <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>107</v>
@@ -1645,7 +1648,7 @@
         <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
         <v>108</v>
@@ -1662,13 +1665,13 @@
         <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E4" t="s">
         <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1683,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,87 +1700,89 @@
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2" spans="1:6" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="B2" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+        <v>117</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+        <v>118</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+        <v>119</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+        <v>120</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+        <v>232</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+        <v>233</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
@@ -1787,9 +1792,11 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="6" t="s">
+        <v>253</v>
+      </c>
       <c r="B10" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>41</v>
@@ -1806,42 +1813,42 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1849,11 +1856,11 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1863,7 +1870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -1883,10 +1890,10 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>235</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>236</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -1897,52 +1904,52 @@
       <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35" t="s">
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="AL1" s="35"/>
+      <c r="AL1" s="38"/>
     </row>
     <row r="2" spans="1:38" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>237</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>238</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
@@ -2055,10 +2062,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>240</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>86</v>
@@ -2502,7 +2509,7 @@
         <v>82</v>
       </c>
       <c r="AL6" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="34" x14ac:dyDescent="0.2">
@@ -2922,7 +2929,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -5842,72 +5849,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
         <v>134</v>
       </c>
-      <c r="C3" t="s">
-        <v>135</v>
-      </c>
       <c r="D3" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5934,36 +5941,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -5990,25 +5997,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>165</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -6016,22 +6023,22 @@
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -6039,22 +6046,22 @@
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -6064,14 +6071,14 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -6081,14 +6088,14 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -6098,14 +6105,14 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -6115,14 +6122,14 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -6132,14 +6139,14 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -6149,14 +6156,14 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -6166,14 +6173,14 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -6183,14 +6190,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -6200,14 +6207,14 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -6217,14 +6224,14 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6508,54 +6515,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>